<commit_message>
feat: cambiar archivo template migración
</commit_message>
<xml_diff>
--- a/src/assets/files/TemplateMigration.xlsx
+++ b/src/assets/files/TemplateMigration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria.gonzalez\Desktop\MisCosas\Concesur\Concenet\Desarrollo\Migrations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF8E376-E2B9-442B-A775-9B51B32682C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D35F434-D6FF-4A45-82E2-98C40226D0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{17C47C1A-1AD3-4394-8AEA-2500455D18C9}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>id_ficha</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>02</t>
+  </si>
+  <si>
+    <t>123XX</t>
+  </si>
+  <si>
+    <t>456XX</t>
   </si>
 </sst>
 </file>
@@ -337,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -355,6 +361,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -672,7 +679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F838ABF-69E7-4C86-88E9-047EC46B2B9F}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -689,7 +698,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -730,6 +739,9 @@
       <c r="B2" s="5">
         <v>1</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="E2" s="5">
         <v>1</v>
       </c>
@@ -758,6 +770,9 @@
       </c>
       <c r="B3" s="5">
         <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>75</v>
@@ -5391,7 +5406,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B72810-D862-407F-B147-1AF128947F2D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5412,7 +5429,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>